<commit_message>
Filled up some missing accuracies for Levenshtein Predictor
</commit_message>
<xml_diff>
--- a/CPT+_accur_variance.xlsx
+++ b/CPT+_accur_variance.xlsx
@@ -1488,8 +1488,14 @@
                 <c:pt idx="2">
                   <c:v>0.62</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.36</c:v>
@@ -3113,8 +3119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="109" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="107" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3444,7 +3450,9 @@
       <c r="D42" s="3">
         <v>0.22</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="3">
+        <v>0.22</v>
+      </c>
       <c r="F42" s="3">
         <v>0.28999999999999998</v>
       </c>
@@ -3506,7 +3514,9 @@
       <c r="D44" s="3">
         <v>0.37</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3">
+        <v>0.2</v>
+      </c>
       <c r="F44" s="3">
         <v>0.34</v>
       </c>

</xml_diff>

<commit_message>
Modified (perhaps) the CPT+_accur_variance.xlsx
</commit_message>
<xml_diff>
--- a/CPT+_accur_variance.xlsx
+++ b/CPT+_accur_variance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Dataset</t>
   </si>
@@ -124,6 +124,12 @@
   <si>
     <t>Levens Pred</t>
   </si>
+  <si>
+    <t>Worst Place</t>
+  </si>
+  <si>
+    <t>CPT+ rank diff. among predictors accuracy</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +177,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -187,16 +193,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -204,6 +226,13 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -211,6 +240,13 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,11 +513,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="940941088"/>
-        <c:axId val="940934288"/>
+        <c:axId val="-303946864"/>
+        <c:axId val="-396466976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="940941088"/>
+        <c:axId val="-303946864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,7 +560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940934288"/>
+        <c:crossAx val="-396466976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -532,7 +568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="940934288"/>
+        <c:axId val="-396466976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -583,7 +619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940941088"/>
+        <c:crossAx val="-303946864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -1514,11 +1550,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="946270816"/>
-        <c:axId val="946273648"/>
+        <c:axId val="-396427664"/>
+        <c:axId val="-396425184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="946270816"/>
+        <c:axId val="-396427664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="946273648"/>
+        <c:crossAx val="-396425184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1569,7 +1605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="946273648"/>
+        <c:axId val="-396425184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,7 +1656,448 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="946270816"/>
+        <c:crossAx val="-396427664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CPT+ accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> rank</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$69:$A$75</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>BMS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MSNBC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BIBLE_W</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE_C</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>KOSARAK</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$69:$C$75</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPT+ rank diff. among predictors accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$69:$A$75</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>BMS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MSNBC</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BIBLE_W</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE_C</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>KOSARAK</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$69:$D$75</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="100"/>
+        <c:axId val="-270812896"/>
+        <c:axId val="-270811120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-270812896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-270811120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-270811120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-270812896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1781,6 +2258,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2757,6 +3274,511 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2846,6 +3868,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>595660</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>152914</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3117,10 +4171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="107" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="110" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3565,6 +4619,122 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="4">
+        <v>7</v>
+      </c>
+      <c r="C69" s="5">
+        <v>1</v>
+      </c>
+      <c r="D69" s="4">
+        <f>B69-C69</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1</v>
+      </c>
+      <c r="C70" s="5">
+        <v>1</v>
+      </c>
+      <c r="D70" s="4">
+        <f>-(C70-B70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="4">
+        <v>5</v>
+      </c>
+      <c r="C71" s="5">
+        <v>2</v>
+      </c>
+      <c r="D71" s="4">
+        <f>-(C71-B71)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="4">
+        <v>9</v>
+      </c>
+      <c r="C72" s="5">
+        <v>3</v>
+      </c>
+      <c r="D72" s="4">
+        <f>-(C72-B72)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="4">
+        <v>9</v>
+      </c>
+      <c r="C73" s="5">
+        <v>3</v>
+      </c>
+      <c r="D73" s="4">
+        <f>-(C73-B73)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="4">
+        <v>2</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1</v>
+      </c>
+      <c r="D74" s="4">
+        <f>-(C74-B74)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="4">
+        <v>8</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="4">
+        <f>-(C75-B75)</f>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>